<commit_message>
upd china holiday, strange mapping mis-align in china but not aus
Former-commit-id: 641de249594dc4a4717a54e6cbbfbacf05788b16 [formerly 641de249594dc4a4717a54e6cbbfbacf05788b16 [formerly 7464045ed03f0ced7d6e48e2339579e2e7989ecc]]
Former-commit-id: 0abcf4beb577f455c4a7f1909f8f349543e9551d
Former-commit-id: 9e5978f68524408e03ee76239b5b97d24f2ab239
</commit_message>
<xml_diff>
--- a/2019_china_holiday/beijing.xlsx
+++ b/2019_china_holiday/beijing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwang/Dropbox (Sydney Uni)/tidytuesday/2019_china_holiday/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27339203-A208-2544-B592-90BD67FCA69B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698062BC-E2AB-CF49-9B75-535B63A59A77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{8BD28E6A-F4D4-4A4B-9170-D7113F44A491}"/>
+    <workbookView xWindow="35500" yWindow="1320" windowWidth="28800" windowHeight="16460" xr2:uid="{8BD28E6A-F4D4-4A4B-9170-D7113F44A491}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Location</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>清华大学</t>
+  </si>
+  <si>
+    <t>Carslaw building</t>
+  </si>
+  <si>
+    <t>My university office</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90527886-AA60-9C42-B138-0D6EA2F379BF}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="284" zoomScaleNormal="284" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,6 +466,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>